<commit_message>
Tutorial Growth Quantification Ready
</commit_message>
<xml_diff>
--- a/Jupyter/Example_GrowthExp.xlsx
+++ b/Jupyter/Example_GrowthExp.xlsx
@@ -207,7 +207,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,19 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -300,7 +313,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,7 +326,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,11 +342,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1105,124 +1122,124 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1819,124 +1836,124 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2533,124 +2550,124 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3298,109 +3315,109 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4018,109 +4035,109 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4738,109 +4755,109 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4864,301 +4881,320 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.94"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="7" t="n">
         <v>0.06</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="J2" s="1" t="n">
+      <c r="I2" s="7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J2" s="7" t="n">
         <v>0.99</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="7" t="n">
         <v>1.1</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="7" t="n">
         <v>0.99</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="7" t="n">
         <v>0.31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="7" t="n">
         <v>2.2</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="7" t="n">
         <v>0.12</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="J3" s="1" t="n">
+      <c r="I3" s="7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J3" s="7" t="n">
         <v>0.99</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="7" t="n">
         <v>2.1</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="7" t="n">
         <v>0.99</v>
       </c>
-      <c r="N3" s="1" t="n">
+      <c r="N3" s="7" t="n">
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="7" t="n">
         <v>0.16</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="7" t="n">
         <v>0.01</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="7" t="n">
         <v>0.99</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="7" t="n">
         <v>2.6</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="L4" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="M4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="1" t="n">
+      <c r="N4" s="7" t="n">
         <v>0.34</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="9" t="n">
         <v>0.17</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.01</v>
       </c>
-      <c r="J5" s="8" t="n">
+      <c r="J5" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="8" t="n">
+      <c r="K5" s="9" t="n">
         <v>2.9</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="L5" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="M5" s="8" t="n">
+      <c r="M5" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="8" t="n">
+      <c r="N5" s="9" t="n">
         <v>0.33</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="9" t="n">
         <v>0.15</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.01</v>
       </c>
-      <c r="J6" s="8" t="n">
+      <c r="J6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="8" t="n">
+      <c r="K6" s="9" t="n">
         <v>2.4</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="L6" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="M6" s="8" t="n">
+      <c r="M6" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="N6" s="8" t="n">
+      <c r="N6" s="9" t="n">
         <v>0.34</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="G7" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="H7" s="8" t="n">
+      <c r="H7" s="9" t="n">
         <v>0.07</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="7" t="n">
         <v>0.01</v>
       </c>
-      <c r="J7" s="8" t="n">
+      <c r="J7" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="K7" s="8" t="n">
+      <c r="K7" s="9" t="n">
         <v>1.4</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="L7" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="M7" s="8" t="n">
+      <c r="M7" s="9" t="n">
         <v>0.97</v>
       </c>
-      <c r="N7" s="8" t="n">
+      <c r="N7" s="9" t="n">
         <v>0.29</v>
       </c>
     </row>

</xml_diff>